<commit_message>
Pushing latest (updating annotations)
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="38">
   <si>
     <t>Name</t>
   </si>
@@ -130,13 +130,13 @@
     <t>FTPFolderPath</t>
   </si>
   <si>
-    <t>/Journal Entry</t>
-  </si>
-  <si>
     <t>SAP_SID</t>
   </si>
   <si>
     <t>SQLConnectionString</t>
+  </si>
+  <si>
+    <t>JE_SharedFolderPath</t>
   </si>
 </sst>
 </file>
@@ -518,7 +518,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A6" sqref="A6:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -599,14 +599,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B6" t="s">
-        <v>35</v>
-      </c>
-    </row>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
@@ -2720,7 +2713,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2783,22 +2776,36 @@
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" t="s">
         <v>37</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" t="s">
+        <v>34</v>
+      </c>
+    </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
updating changes to use db credentials
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" activeTab="2"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19430" windowHeight="10430" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="40">
   <si>
     <t>Name</t>
   </si>
@@ -137,6 +137,13 @@
   </si>
   <si>
     <t>JE_SharedFolderPath</t>
+  </si>
+  <si>
+    <t>SAP_ServiceID_JournalEntry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SQL_Credential
+</t>
   </si>
 </sst>
 </file>
@@ -518,15 +525,15 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:B6"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5703125" customWidth="1"/>
+    <col min="1" max="1" width="43.54296875" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="81.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -582,12 +589,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="18.95" customHeight="1">
+    <row r="4" spans="1:26" ht="19" customHeight="1">
       <c r="A4" s="5" t="s">
         <v>30</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="C4" s="4"/>
     </row>
@@ -599,7 +606,14 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1604,12 +1618,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="75.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1646,7 +1660,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="30">
+    <row r="2" spans="1:26" ht="29">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2713,15 +2727,15 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" customWidth="1"/>
-    <col min="3" max="3" width="60.28515625" customWidth="1"/>
-    <col min="4" max="26" width="65.42578125" customWidth="1"/>
+    <col min="1" max="1" width="31.81640625" customWidth="1"/>
+    <col min="2" max="2" width="30.1796875" customWidth="1"/>
+    <col min="3" max="3" width="60.26953125" customWidth="1"/>
+    <col min="4" max="26" width="65.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>